<commit_message>
change in lingo sheet
</commit_message>
<xml_diff>
--- a/Data/ExLingo.xlsx
+++ b/Data/ExLingo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="9345" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="9345" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Final (2)" sheetId="7" r:id="rId1"/>
@@ -19,13 +19,13 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final (2)'!$A$1:$K$403</definedName>
-    <definedName name="ct">Lingo!$D$1:$D$4</definedName>
+    <definedName name="ct">Lingo!$D$1:$D$9</definedName>
     <definedName name="emp">Target!$B$3</definedName>
-    <definedName name="gni">Lingo!$E$1:$E$4</definedName>
-    <definedName name="pl">Lingo!$I$1:$I$4</definedName>
-    <definedName name="pli">Lingo!$G$1:$G$4</definedName>
-    <definedName name="pm">Lingo!$J$1:$J$4</definedName>
-    <definedName name="pu">Lingo!$K$1:$K$4</definedName>
+    <definedName name="gni">Lingo!$E$1:$E$9</definedName>
+    <definedName name="pl">Lingo!$I$1:$I$9</definedName>
+    <definedName name="pli">Lingo!$G$1:$G$9</definedName>
+    <definedName name="pm">Lingo!$J$1:$J$9</definedName>
+    <definedName name="pu">Lingo!$K$1:$K$9</definedName>
     <definedName name="rev">Target!$B$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="692">
   <si>
     <t>N</t>
   </si>
@@ -2532,8 +2532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K403"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A159" sqref="A159:XFD159"/>
+    <sheetView topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194:XFD196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16760,7 +16760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -16770,10 +16770,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16815,19 +16815,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D2" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E2" s="17">
-        <v>47260</v>
+        <v>4280</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>147</v>
@@ -16836,33 +16836,33 @@
         <v>2</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="I2" s="21">
-        <v>7.6776669196152352E-3</v>
+        <v>3.0046654905444739E-2</v>
       </c>
       <c r="J2" s="11">
-        <v>2.9815233273297551E-2</v>
+        <v>3.9398905394853467E-2</v>
       </c>
       <c r="K2" s="19">
-        <v>6.2950946325533164E-2</v>
+        <v>4.9039962524983639E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
-        <v>138</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D3" s="12">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E3" s="17">
-        <v>18320</v>
+        <v>4280</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>149</v>
@@ -16871,51 +16871,226 @@
         <v>3</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>430</v>
+        <v>301</v>
       </c>
       <c r="I3" s="21">
-        <v>0.13558370993750485</v>
+        <v>3.1775252121018109E-2</v>
       </c>
       <c r="J3" s="11">
-        <v>0.13966594784360642</v>
+        <v>7.772686245920965E-2</v>
       </c>
       <c r="K3" s="19">
-        <v>0.14374818574970799</v>
+        <v>0.17564667785103982</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
-        <v>155</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="E4" s="17">
+        <v>60050</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="20">
+        <v>3</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="I4" s="21">
+        <v>4.8407014117393857E-2</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0.1278324518399418</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0.23334164580493164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="17">
+        <v>47260</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="20">
+        <v>2</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="I5" s="21">
+        <v>7.6776669196152352E-3</v>
+      </c>
+      <c r="J5" s="11">
+        <v>2.9815233273297551E-2</v>
+      </c>
+      <c r="K5" s="19">
+        <v>6.2950946325533164E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="17">
+        <v>47260</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="20">
+        <v>1</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="I6" s="21">
+        <v>8.1714734218456569E-2</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0.11700606768122054</v>
+      </c>
+      <c r="K6" s="19">
+        <v>0.15229740114398455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
         <v>193</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0.29649999999999999</v>
-      </c>
-      <c r="E4" s="17">
-        <v>45790</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="B7" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E7" s="17">
+        <v>32830</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="20">
+        <v>2</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>488</v>
+      </c>
+      <c r="I7" s="21">
+        <v>9.5958740467727392E-3</v>
+      </c>
+      <c r="J7" s="11">
+        <v>2.000235955350866E-2</v>
+      </c>
+      <c r="K7" s="19">
+        <v>4.0666996611319353E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>194</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E8" s="17">
+        <v>32830</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G8" s="20">
         <v>1</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>408</v>
-      </c>
-      <c r="I4" s="21">
-        <v>6.4999123976238193E-2</v>
-      </c>
-      <c r="J4" s="11">
-        <v>8.3671628180126287E-2</v>
-      </c>
-      <c r="K4" s="19">
-        <v>0.12792944909661313</v>
+      <c r="H8" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="I8" s="21">
+        <v>3.972062576059085E-2</v>
+      </c>
+      <c r="J8" s="11">
+        <v>6.1999169361979495E-2</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.10827656744114039</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>195</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E9" s="17">
+        <v>32830</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="20">
+        <v>3</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="I9" s="21">
+        <v>2.191384689688711E-2</v>
+      </c>
+      <c r="J9" s="11">
+        <v>4.8206183032513075E-2</v>
+      </c>
+      <c r="K9" s="19">
+        <v>9.9721619084336896E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major change in the model
</commit_message>
<xml_diff>
--- a/Data/ExLingo.xlsx
+++ b/Data/ExLingo.xlsx
@@ -19,13 +19,13 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final (2)'!$A$1:$K$403</definedName>
-    <definedName name="ct">Lingo!$D$1:$D$9</definedName>
+    <definedName name="ct">Lingo!$D$1:$D$6</definedName>
     <definedName name="emp">Target!$B$3</definedName>
-    <definedName name="gni">Lingo!$E$1:$E$9</definedName>
-    <definedName name="pl">Lingo!$I$1:$I$9</definedName>
-    <definedName name="pli">Lingo!$G$1:$G$9</definedName>
-    <definedName name="pm">Lingo!$J$1:$J$9</definedName>
-    <definedName name="pu">Lingo!$K$1:$K$9</definedName>
+    <definedName name="gni">Lingo!$E$1:$E$6</definedName>
+    <definedName name="pl">Lingo!$I$1:$I$6</definedName>
+    <definedName name="pli">Lingo!$G$1:$G$6</definedName>
+    <definedName name="pm">Lingo!$J$1:$J$6</definedName>
+    <definedName name="pu">Lingo!$K$1:$K$6</definedName>
     <definedName name="rev">Target!$B$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="692">
   <si>
     <t>N</t>
   </si>
@@ -16770,10 +16770,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16885,211 +16885,106 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
-        <v>27</v>
+        <v>193</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0.3</v>
+        <v>74</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.27900000000000003</v>
       </c>
       <c r="E4" s="17">
-        <v>60050</v>
+        <v>32830</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G4" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>316</v>
+        <v>488</v>
       </c>
       <c r="I4" s="21">
-        <v>4.8407014117393857E-2</v>
+        <v>9.5958740467727392E-3</v>
       </c>
       <c r="J4" s="11">
-        <v>0.1278324518399418</v>
+        <v>2.000235955350866E-2</v>
       </c>
       <c r="K4" s="19">
-        <v>0.23334164580493164</v>
+        <v>4.0666996611319353E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <v>28</v>
+        <v>194</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.25</v>
+        <v>74</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.27900000000000003</v>
       </c>
       <c r="E5" s="17">
-        <v>47260</v>
+        <v>32830</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G5" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>317</v>
+        <v>489</v>
       </c>
       <c r="I5" s="21">
-        <v>7.6776669196152352E-3</v>
+        <v>3.972062576059085E-2</v>
       </c>
       <c r="J5" s="11">
-        <v>2.9815233273297551E-2</v>
+        <v>6.1999169361979495E-2</v>
       </c>
       <c r="K5" s="19">
-        <v>6.2950946325533164E-2</v>
+        <v>0.10827656744114039</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.25</v>
+        <v>74</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.27900000000000003</v>
       </c>
       <c r="E6" s="17">
-        <v>47260</v>
+        <v>32830</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G6" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>318</v>
+        <v>490</v>
       </c>
       <c r="I6" s="21">
-        <v>8.1714734218456569E-2</v>
+        <v>2.191384689688711E-2</v>
       </c>
       <c r="J6" s="11">
-        <v>0.11700606768122054</v>
+        <v>4.8206183032513075E-2</v>
       </c>
       <c r="K6" s="19">
-        <v>0.15229740114398455</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>193</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="E7" s="17">
-        <v>32830</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" s="20">
-        <v>2</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>488</v>
-      </c>
-      <c r="I7" s="21">
-        <v>9.5958740467727392E-3</v>
-      </c>
-      <c r="J7" s="11">
-        <v>2.000235955350866E-2</v>
-      </c>
-      <c r="K7" s="19">
-        <v>4.0666996611319353E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>194</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="E8" s="17">
-        <v>32830</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G8" s="20">
-        <v>1</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>489</v>
-      </c>
-      <c r="I8" s="21">
-        <v>3.972062576059085E-2</v>
-      </c>
-      <c r="J8" s="11">
-        <v>6.1999169361979495E-2</v>
-      </c>
-      <c r="K8" s="19">
-        <v>0.10827656744114039</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>195</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="E9" s="17">
-        <v>32830</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G9" s="20">
-        <v>3</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>490</v>
-      </c>
-      <c r="I9" s="21">
-        <v>2.191384689688711E-2</v>
-      </c>
-      <c r="J9" s="11">
-        <v>4.8206183032513075E-2</v>
-      </c>
-      <c r="K9" s="19">
         <v>9.9721619084336896E-2</v>
       </c>
     </row>

</xml_diff>